<commit_message>
Actualización plantilla de tareas iteración 4
Ae actualizaron errores en la plantilla de tareas.
</commit_message>
<xml_diff>
--- a/Documentos/Tareas/Iteración_4.xlsx
+++ b/Documentos/Tareas/Iteración_4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raymu\Desktop\ProyectoDesarrolloSW-EQ1\Documentos\Tareas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B8035E3-7D6E-419C-A82B-BDB3A8FB7D58}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66B057A6-AB77-4CC5-9EE7-79617250D3AD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -434,12 +434,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -466,6 +460,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -805,7 +805,7 @@
       <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomRight" activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -880,84 +880,84 @@
       </c>
     </row>
     <row r="4" spans="2:53" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H4" s="15" t="s">
+      <c r="H4" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="16"/>
+      <c r="I4" s="25"/>
       <c r="J4" s="9"/>
-      <c r="K4" s="15" t="s">
+      <c r="K4" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="16"/>
+      <c r="L4" s="25"/>
       <c r="M4" s="9"/>
-      <c r="N4" s="15" t="s">
+      <c r="N4" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="O4" s="16"/>
+      <c r="O4" s="25"/>
       <c r="P4" s="9"/>
-      <c r="Q4" s="15" t="s">
+      <c r="Q4" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="R4" s="16"/>
+      <c r="R4" s="25"/>
       <c r="S4" s="9"/>
-      <c r="T4" s="15" t="s">
+      <c r="T4" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="U4" s="16"/>
+      <c r="U4" s="25"/>
       <c r="V4" s="9"/>
-      <c r="W4" s="15" t="s">
+      <c r="W4" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="X4" s="16"/>
+      <c r="X4" s="25"/>
       <c r="Y4" s="9"/>
-      <c r="Z4" s="15" t="s">
+      <c r="Z4" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="AA4" s="16"/>
+      <c r="AA4" s="25"/>
       <c r="AB4" s="9"/>
-      <c r="AC4" s="15" t="s">
+      <c r="AC4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="AD4" s="16"/>
+      <c r="AD4" s="25"/>
       <c r="AE4" s="9"/>
-      <c r="AF4" s="15" t="s">
+      <c r="AF4" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="AG4" s="16"/>
+      <c r="AG4" s="25"/>
       <c r="AH4" s="9"/>
-      <c r="AI4" s="15" t="s">
+      <c r="AI4" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="AJ4" s="16"/>
+      <c r="AJ4" s="25"/>
       <c r="AK4" s="9"/>
-      <c r="AL4" s="15" t="s">
+      <c r="AL4" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="AM4" s="16"/>
+      <c r="AM4" s="25"/>
       <c r="AN4" s="9"/>
-      <c r="AO4" s="15" t="s">
+      <c r="AO4" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="AP4" s="16"/>
+      <c r="AP4" s="25"/>
       <c r="AQ4" s="9"/>
-      <c r="AR4" s="15" t="s">
+      <c r="AR4" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="AS4" s="16"/>
+      <c r="AS4" s="25"/>
       <c r="AT4" s="9"/>
-      <c r="AU4" s="15" t="s">
+      <c r="AU4" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="AV4" s="16"/>
+      <c r="AV4" s="25"/>
       <c r="AW4" s="9"/>
-      <c r="AX4" s="15" t="s">
+      <c r="AX4" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="AY4" s="16"/>
-      <c r="AZ4" s="15" t="s">
+      <c r="AY4" s="25"/>
+      <c r="AZ4" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="BA4" s="16"/>
+      <c r="BA4" s="25"/>
     </row>
     <row r="5" spans="2:53" ht="45" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
@@ -1090,19 +1090,19 @@
       </c>
     </row>
     <row r="6" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="E6" s="20" t="s">
+      <c r="E6" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="20"/>
+      <c r="F6" s="18"/>
       <c r="G6" s="14">
         <v>4</v>
       </c>
@@ -1209,15 +1209,15 @@
       </c>
     </row>
     <row r="7" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B7" s="19"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20" t="s">
+      <c r="B7" s="17"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F7" s="20"/>
+      <c r="F7" s="18"/>
       <c r="G7" s="14">
         <v>2</v>
       </c>
@@ -1324,15 +1324,15 @@
       </c>
     </row>
     <row r="8" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B8" s="19"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20" t="s">
+      <c r="B8" s="17"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="E8" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F8" s="20"/>
+      <c r="F8" s="18"/>
       <c r="G8" s="14">
         <v>1</v>
       </c>
@@ -1441,11 +1441,11 @@
       <c r="C9" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="D9" s="22" t="s">
         <v>46</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F9" s="22"/>
       <c r="G9" s="14">
@@ -1552,11 +1552,11 @@
     <row r="10" spans="2:53" x14ac:dyDescent="0.25">
       <c r="B10" s="21"/>
       <c r="C10" s="22"/>
-      <c r="D10" s="25" t="s">
+      <c r="D10" s="22" t="s">
         <v>45</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F10" s="22"/>
       <c r="G10" s="14">
@@ -1669,11 +1669,11 @@
     <row r="11" spans="2:53" x14ac:dyDescent="0.25">
       <c r="B11" s="21"/>
       <c r="C11" s="22"/>
-      <c r="D11" s="25" t="s">
+      <c r="D11" s="22" t="s">
         <v>47</v>
       </c>
       <c r="E11" s="22" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F11" s="22"/>
       <c r="G11" s="14">
@@ -1782,19 +1782,19 @@
       </c>
     </row>
     <row r="12" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="D12" s="24" t="s">
+      <c r="D12" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="E12" s="24" t="s">
+      <c r="E12" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="F12" s="24"/>
+      <c r="F12" s="22"/>
       <c r="G12" s="14">
         <v>8</v>
       </c>
@@ -1897,15 +1897,15 @@
       </c>
     </row>
     <row r="13" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B13" s="23"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24" t="s">
+      <c r="B13" s="21"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="24" t="s">
+      <c r="E13" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="F13" s="24"/>
+      <c r="F13" s="22"/>
       <c r="G13" s="14">
         <v>2</v>
       </c>
@@ -2008,15 +2008,15 @@
       </c>
     </row>
     <row r="14" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B14" s="23"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24" t="s">
+      <c r="B14" s="21"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="E14" s="24" t="s">
+      <c r="E14" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="F14" s="24"/>
+      <c r="F14" s="22"/>
       <c r="G14" s="14">
         <v>2</v>
       </c>
@@ -2119,19 +2119,19 @@
       </c>
     </row>
     <row r="15" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="C15" s="22" t="s">
+      <c r="C15" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="D15" s="25" t="s">
+      <c r="D15" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="E15" s="22" t="s">
+      <c r="E15" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="F15" s="22"/>
+      <c r="F15" s="20"/>
       <c r="G15" s="14">
         <v>6</v>
       </c>
@@ -2234,15 +2234,15 @@
       </c>
     </row>
     <row r="16" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B16" s="21"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="25" t="s">
+      <c r="B16" s="19"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="E16" s="22" t="s">
+      <c r="E16" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="F16" s="22"/>
+      <c r="F16" s="20"/>
       <c r="G16" s="14">
         <v>2</v>
       </c>
@@ -2349,15 +2349,15 @@
       </c>
     </row>
     <row r="17" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B17" s="21"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="25" t="s">
+      <c r="B17" s="19"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="E17" s="22" t="s">
+      <c r="E17" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="F17" s="22"/>
+      <c r="F17" s="20"/>
       <c r="G17" s="14">
         <v>1</v>
       </c>
@@ -2464,19 +2464,19 @@
       </c>
     </row>
     <row r="18" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C18" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="D18" s="20" t="s">
+      <c r="D18" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="E18" s="20" t="s">
+      <c r="E18" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F18" s="20"/>
+      <c r="F18" s="18"/>
       <c r="G18" s="14">
         <v>5</v>
       </c>
@@ -2583,15 +2583,15 @@
       </c>
     </row>
     <row r="19" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B19" s="19"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20" t="s">
+      <c r="B19" s="17"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="E19" s="20" t="s">
+      <c r="E19" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F19" s="20"/>
+      <c r="F19" s="18"/>
       <c r="G19" s="14">
         <v>2</v>
       </c>
@@ -2698,15 +2698,15 @@
       </c>
     </row>
     <row r="20" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B20" s="19"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20" t="s">
+      <c r="B20" s="17"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="E20" s="20" t="s">
+      <c r="E20" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F20" s="20"/>
+      <c r="F20" s="18"/>
       <c r="G20" s="14">
         <v>1</v>
       </c>
@@ -2809,19 +2809,19 @@
       </c>
     </row>
     <row r="21" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B21" s="21" t="s">
+      <c r="B21" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="C21" s="22" t="s">
+      <c r="C21" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="D21" s="25" t="s">
+      <c r="D21" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="E21" s="22" t="s">
+      <c r="E21" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="F21" s="22"/>
+      <c r="F21" s="20"/>
       <c r="G21" s="14">
         <v>4</v>
       </c>
@@ -2924,15 +2924,15 @@
       </c>
     </row>
     <row r="22" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B22" s="21"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="25" t="s">
+      <c r="B22" s="19"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="E22" s="22" t="s">
+      <c r="E22" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="F22" s="22"/>
+      <c r="F22" s="20"/>
       <c r="G22" s="14">
         <v>2</v>
       </c>
@@ -3035,15 +3035,15 @@
       </c>
     </row>
     <row r="23" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B23" s="21"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="25" t="s">
+      <c r="B23" s="19"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="E23" s="22" t="s">
+      <c r="E23" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="F23" s="22"/>
+      <c r="F23" s="20"/>
       <c r="G23" s="14">
         <v>1</v>
       </c>
@@ -3146,19 +3146,19 @@
       </c>
     </row>
     <row r="24" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B24" s="19" t="s">
+      <c r="B24" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="C24" s="20" t="s">
+      <c r="C24" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="D24" s="20" t="s">
+      <c r="D24" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="E24" s="20" t="s">
+      <c r="E24" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F24" s="20"/>
+      <c r="F24" s="18"/>
       <c r="G24" s="14">
         <v>4</v>
       </c>
@@ -3263,15 +3263,15 @@
       </c>
     </row>
     <row r="25" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B25" s="19"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20" t="s">
+      <c r="B25" s="17"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="E25" s="20" t="s">
+      <c r="E25" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F25" s="20"/>
+      <c r="F25" s="18"/>
       <c r="G25" s="14">
         <v>2</v>
       </c>
@@ -3376,15 +3376,15 @@
       </c>
     </row>
     <row r="26" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B26" s="19"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20" t="s">
+      <c r="B26" s="17"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="E26" s="20" t="s">
+      <c r="E26" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F26" s="20"/>
+      <c r="F26" s="18"/>
       <c r="G26" s="14">
         <v>1</v>
       </c>
@@ -3592,15 +3592,15 @@
       </c>
     </row>
     <row r="28" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B28" s="19"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20" t="s">
+      <c r="B28" s="17"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="E28" s="20" t="s">
+      <c r="E28" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F28" s="20"/>
+      <c r="F28" s="18"/>
       <c r="G28" s="14">
         <v>4</v>
       </c>
@@ -3816,15 +3816,15 @@
       </c>
     </row>
     <row r="30" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B30" s="17"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18" t="s">
+      <c r="B30" s="15"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="E30" s="18" t="s">
+      <c r="E30" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="F30" s="18"/>
+      <c r="F30" s="16"/>
       <c r="G30" s="14">
         <v>1</v>
       </c>
@@ -3931,15 +3931,15 @@
       </c>
     </row>
     <row r="31" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B31" s="17"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18" t="s">
+      <c r="B31" s="15"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="E31" s="18" t="s">
+      <c r="E31" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="F31" s="18"/>
+      <c r="F31" s="16"/>
       <c r="G31" s="14">
         <v>1</v>
       </c>

</xml_diff>